<commit_message>
SE-341 Added handling of transcriptomics and proteomics data.
SVN: 21606
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/OD600-Example.xlsx
+++ b/eu_basynthec/sourceTest/examples/OD600-Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="8100" windowWidth="27520" windowHeight="12740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1280" yWindow="8100" windowWidth="27520" windowHeight="12740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="openbis-metadata" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -651,7 +651,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -670,7 +669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -812,7 +811,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
LMS-2340 Updating basynthec stuff based on results of the leiden meeting.
SVN: 21872
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/OD600-Example.xlsx
+++ b/eu_basynthec/sourceTest/examples/OD600-Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="8100" windowWidth="27520" windowHeight="12740" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24720" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="openbis-metadata" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>One of Lin, Log2, Log10, or Ln</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,79 +57,79 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Value Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scale</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The openBIS experiment identifier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>One of Value, Mean, Median, Std, Var, Error, or Iqr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/TEST/TEST/TEST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value Unit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dimensionless</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Must be Dimensionless</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OD600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Strain</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Value Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Scale</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The openBIS experiment identifier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The Strain Id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>One of Value, Mean, Median, Std, Var, Error, or Iqr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Abs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/TEST/TEST/TEST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>strain1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value Unit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dimensionless</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Must be Dimensionless</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OD600</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OD600</t>
+    <t>MGP100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MGP20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MGP1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MGP999</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -549,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -567,7 +567,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>3</v>
@@ -578,82 +578,70 @@
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="3" max="1048575" man="1"/>
   </colBreaks>
@@ -667,10 +655,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -682,7 +670,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -747,10 +735,10 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <v>0.05</v>
@@ -807,6 +795,201 @@
         <v>2.09</v>
       </c>
       <c r="U2">
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>0.05</v>
+      </c>
+      <c r="D3">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="E3">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="F3">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.107</v>
+      </c>
+      <c r="H3">
+        <v>0.127</v>
+      </c>
+      <c r="I3">
+        <v>0.155</v>
+      </c>
+      <c r="J3">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="K3">
+        <v>0.24</v>
+      </c>
+      <c r="L3">
+        <v>0.33</v>
+      </c>
+      <c r="M3">
+        <v>0.43</v>
+      </c>
+      <c r="N3">
+        <v>0.49</v>
+      </c>
+      <c r="O3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="P3">
+        <v>0.66</v>
+      </c>
+      <c r="Q3">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="R3">
+        <v>1.42</v>
+      </c>
+      <c r="S3">
+        <v>1.49</v>
+      </c>
+      <c r="T3">
+        <v>2.09</v>
+      </c>
+      <c r="U3">
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>0.05</v>
+      </c>
+      <c r="D4">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="E4">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="F4">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="G4">
+        <v>0.107</v>
+      </c>
+      <c r="H4">
+        <v>0.127</v>
+      </c>
+      <c r="I4">
+        <v>0.155</v>
+      </c>
+      <c r="J4">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="K4">
+        <v>0.24</v>
+      </c>
+      <c r="L4">
+        <v>0.33</v>
+      </c>
+      <c r="M4">
+        <v>0.43</v>
+      </c>
+      <c r="N4">
+        <v>0.49</v>
+      </c>
+      <c r="O4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="P4">
+        <v>0.66</v>
+      </c>
+      <c r="Q4">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="R4">
+        <v>1.42</v>
+      </c>
+      <c r="S4">
+        <v>1.49</v>
+      </c>
+      <c r="T4">
+        <v>2.09</v>
+      </c>
+      <c r="U4">
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>0.05</v>
+      </c>
+      <c r="D5">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="E5">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="F5">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="G5">
+        <v>0.107</v>
+      </c>
+      <c r="H5">
+        <v>0.127</v>
+      </c>
+      <c r="I5">
+        <v>0.155</v>
+      </c>
+      <c r="J5">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="K5">
+        <v>0.24</v>
+      </c>
+      <c r="L5">
+        <v>0.33</v>
+      </c>
+      <c r="M5">
+        <v>0.43</v>
+      </c>
+      <c r="N5">
+        <v>0.49</v>
+      </c>
+      <c r="O5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="P5">
+        <v>0.66</v>
+      </c>
+      <c r="Q5">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="R5">
+        <v>1.42</v>
+      </c>
+      <c r="S5">
+        <v>1.49</v>
+      </c>
+      <c r="T5">
+        <v>2.09</v>
+      </c>
+      <c r="U5">
         <v>3.22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
LMS-2391 Split TSV files where necessary. Switched tab to spaces in all python code.
SVN: 22070
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/OD600-Example.xlsx
+++ b/eu_basynthec/sourceTest/examples/OD600-Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24720" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24720" windowHeight="16740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="openbis-metadata" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>One of Lin, Log2, Log10, or Ln</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -551,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -655,10 +655,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -993,9 +993,75 @@
         <v>3.22</v>
       </c>
     </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>0.05</v>
+      </c>
+      <c r="D6">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="E6">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="F6">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.107</v>
+      </c>
+      <c r="H6">
+        <v>0.127</v>
+      </c>
+      <c r="I6">
+        <v>0.155</v>
+      </c>
+      <c r="J6">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="K6">
+        <v>0.24</v>
+      </c>
+      <c r="L6">
+        <v>0.33</v>
+      </c>
+      <c r="M6">
+        <v>0.43</v>
+      </c>
+      <c r="N6">
+        <v>0.49</v>
+      </c>
+      <c r="O6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="P6">
+        <v>0.66</v>
+      </c>
+      <c r="Q6">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="R6">
+        <v>1.42</v>
+      </c>
+      <c r="S6">
+        <v>1.49</v>
+      </c>
+      <c r="T6">
+        <v>2.09</v>
+      </c>
+      <c r="U6">
+        <v>3.22</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
MINOR: Fix the example to refer to strains by their correct name
SVN: 24013
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/OD600-Example.xlsx
+++ b/eu_basynthec/sourceTest/examples/OD600-Example.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21105"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
@@ -117,15 +117,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>JJS-MGP1</t>
-  </si>
-  <si>
     <t>JJS-MGP100</t>
   </si>
   <si>
-    <t>JJS-MGP20</t>
-  </si>
-  <si>
     <t>JJS-MGP999</t>
   </si>
   <si>
@@ -133,6 +127,12 @@
   </si>
   <si>
     <t>WT 168 trp+</t>
+  </si>
+  <si>
+    <t>JJS-MGP001</t>
+  </si>
+  <si>
+    <t>JJS-MGP020</t>
   </si>
 </sst>
 </file>
@@ -680,7 +680,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -757,7 +757,7 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>

</xml_diff>